<commit_message>
Dum day - but all is back to normal
</commit_message>
<xml_diff>
--- a/output/sites/test_differences_sites_nut_all_scats.xlsx
+++ b/output/sites/test_differences_sites_nut_all_scats.xlsx
@@ -383,22 +383,22 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.919</v>
+        <v>0.93</v>
       </c>
       <c r="B2" t="n">
-        <v>0.979</v>
+        <v>0.977</v>
       </c>
       <c r="C2" t="n">
         <v>0.934</v>
       </c>
       <c r="D2" t="n">
-        <v>0.923</v>
+        <v>0.934</v>
       </c>
       <c r="E2" t="n">
-        <v>0.944</v>
+        <v>0.95</v>
       </c>
       <c r="F2" t="n">
-        <v>0.92</v>
+        <v>0.938</v>
       </c>
     </row>
   </sheetData>

</xml_diff>